<commit_message>
Message boxes - Terminar
</commit_message>
<xml_diff>
--- a/TP1_GRUPO X.xlsx
+++ b/TP1_GRUPO X.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blakz\OneDrive\Documentos\AyPII TP1\AyP2-mod2-TP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba58f79a5dcad87f/Escritorio/facultad/materias/Acústica y Psicoacústica II/AyP2-mod2-TP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD8D89-CB9B-4F34-9CA0-2AEE798AD357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{D5CD8D89-CB9B-4F34-9CA0-2AEE798AD357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5FD4AAD-AB77-45C8-994B-D9961A1B0247}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PYL_6.0_4.0_12.5" sheetId="1" r:id="rId1"/>
@@ -2352,15 +2352,15 @@
   <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:32" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>45.18</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>47.72</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>44.93</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>46.97</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -3053,7 +3053,7 @@
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3125,7 +3125,7 @@
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>45.18</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>47.72</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>44.93</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Mas correcciones de errores
</commit_message>
<xml_diff>
--- a/TP1_GRUPO X.xlsx
+++ b/TP1_GRUPO X.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba58f79a5dcad87f/Escritorio/facultad/materias/Acústica y Psicoacústica II/AyP2-mod2-TP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{D5CD8D89-CB9B-4F34-9CA0-2AEE798AD357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5FD4AAD-AB77-45C8-994B-D9961A1B0247}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{D5CD8D89-CB9B-4F34-9CA0-2AEE798AD357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C9EED62-E9F3-44DC-B3A0-278D747B2571}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PYL_6.0_4.0_12.5" sheetId="1" r:id="rId1"/>
+    <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>SHARP</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>DIFERENCIA</t>
-  </si>
-  <si>
-    <t>PYL</t>
   </si>
 </sst>
 </file>
@@ -255,7 +252,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$6:$AF$6</c:f>
+              <c:f>Plantilla!$B$6:$AF$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -357,103 +354,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$7:$AF$7</c:f>
+              <c:f>Plantilla!$B$7:$AF$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>-0.98</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.97</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.04</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.98</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.99</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.06</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.94</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17.079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>19.02</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20.96</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.97</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25.04</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>26.98</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>28.99</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>31.06</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>34.94</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>37.08</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>39.020000000000003</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>40.96</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>42.97</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>18.18</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>23.57</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>27.9</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>31.85</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>35.28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>38.56</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>42.07</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>45.18</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -484,7 +388,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$6:$AF$6</c:f>
+              <c:f>Plantilla!$B$6:$AF$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -586,103 +490,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$8:$AF$8</c:f>
+              <c:f>Plantilla!$B$8:$AF$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>-0.17</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.28</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.94</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.7699999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.56</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.4600000000000009</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.47</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.28</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.41</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18.34</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20.27</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.27</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>26.28</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>28.29</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30.36</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>32.299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>34.24</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>36.29</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>33.17</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>29.28</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>24.22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>26.88</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>29.76</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>32.75</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>35.840000000000003</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>38.729999999999997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>41.63</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44.83</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>47.72</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -713,7 +524,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$6:$AF$6</c:f>
+              <c:f>Plantilla!$B$6:$AF$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -815,103 +626,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$9:$AF$9</c:f>
+              <c:f>Plantilla!$B$9:$AF$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>8.0500000000000007</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.08</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.59</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.43</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.43</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.61</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.95</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.27</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.65</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17.22</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18.66</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20.11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21.61</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>23.14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>24.54</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>25.95</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>27.32</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28.49</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>29.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30.32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>30.55</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>29.64</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>20.21</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>22.78</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>30.57</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>33.89</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>36.79</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>39.549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>42.45</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44.93</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -927,7 +645,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$A$10</c:f>
+              <c:f>Plantilla!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -950,7 +668,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$6:$AF$6</c:f>
+              <c:f>Plantilla!$B$6:$AF$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -1052,103 +770,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PYL_6.0_4.0_12.5'!$B$10:$AF$10</c:f>
+              <c:f>Plantilla!$B$10:$AF$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.98</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.59</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.04</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.59</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.64</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17.39</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18.989999999999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20.62</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.33</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.12</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25.8</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27.75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>29.81</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>31.74</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>33.659999999999997</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>35.76</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>37.57</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>38.78</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>16.91</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>20.86</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25.36</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>29.69</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>33.64</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>37.07</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>40.35</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43.86</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>46.97</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2086,6 +1711,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -2352,7 +1981,7 @@
   <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2364,34 +1993,26 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:32" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
-        <v>6</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
-        <v>4</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
-        <v>12.5</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
@@ -2495,393 +2116,145 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
-        <v>-0.98</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2.97</v>
-      </c>
-      <c r="E7" s="6">
-        <v>5.04</v>
-      </c>
-      <c r="F7" s="6">
-        <v>6.98</v>
-      </c>
-      <c r="G7" s="6">
-        <v>8.99</v>
-      </c>
-      <c r="H7" s="6">
-        <v>11.06</v>
-      </c>
-      <c r="I7" s="6">
-        <v>13</v>
-      </c>
-      <c r="J7" s="6">
-        <v>14.94</v>
-      </c>
-      <c r="K7" s="6">
-        <v>17.079999999999998</v>
-      </c>
-      <c r="L7" s="6">
-        <v>19.02</v>
-      </c>
-      <c r="M7" s="6">
-        <v>20.96</v>
-      </c>
-      <c r="N7" s="6">
-        <v>22.97</v>
-      </c>
-      <c r="O7" s="6">
-        <v>25.04</v>
-      </c>
-      <c r="P7" s="6">
-        <v>26.98</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>28.99</v>
-      </c>
-      <c r="R7" s="6">
-        <v>31.06</v>
-      </c>
-      <c r="S7" s="6">
-        <v>33</v>
-      </c>
-      <c r="T7" s="6">
-        <v>34.94</v>
-      </c>
-      <c r="U7" s="6">
-        <v>37.08</v>
-      </c>
-      <c r="V7" s="6">
-        <v>39.020000000000003</v>
-      </c>
-      <c r="W7" s="6">
-        <v>40.96</v>
-      </c>
-      <c r="X7" s="6">
-        <v>42.97</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>18.18</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>23.57</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>27.9</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>31.85</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>35.28</v>
-      </c>
-      <c r="AD7" s="6">
-        <v>38.56</v>
-      </c>
-      <c r="AE7" s="6">
-        <v>42.07</v>
-      </c>
-      <c r="AF7" s="6">
-        <v>45.18</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6">
-        <v>-0.17</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1.28</v>
-      </c>
-      <c r="D8" s="6">
-        <v>2.94</v>
-      </c>
-      <c r="E8" s="6">
-        <v>4.7699999999999996</v>
-      </c>
-      <c r="F8" s="6">
-        <v>6.56</v>
-      </c>
-      <c r="G8" s="6">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="H8" s="6">
-        <v>10.47</v>
-      </c>
-      <c r="I8" s="6">
-        <v>12.37</v>
-      </c>
-      <c r="J8" s="6">
-        <v>14.28</v>
-      </c>
-      <c r="K8" s="6">
-        <v>16.41</v>
-      </c>
-      <c r="L8" s="6">
-        <v>18.34</v>
-      </c>
-      <c r="M8" s="6">
-        <v>20.27</v>
-      </c>
-      <c r="N8" s="6">
-        <v>22.27</v>
-      </c>
-      <c r="O8" s="6">
-        <v>24.35</v>
-      </c>
-      <c r="P8" s="6">
-        <v>26.28</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>28.29</v>
-      </c>
-      <c r="R8" s="6">
-        <v>30.36</v>
-      </c>
-      <c r="S8" s="6">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="T8" s="6">
-        <v>34.24</v>
-      </c>
-      <c r="U8" s="6">
-        <v>36.29</v>
-      </c>
-      <c r="V8" s="6">
-        <v>33.17</v>
-      </c>
-      <c r="W8" s="6">
-        <v>29.28</v>
-      </c>
-      <c r="X8" s="6">
-        <v>24.22</v>
-      </c>
-      <c r="Y8" s="6">
-        <v>26.88</v>
-      </c>
-      <c r="Z8" s="6">
-        <v>29.76</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>32.75</v>
-      </c>
-      <c r="AB8" s="6">
-        <v>35.840000000000003</v>
-      </c>
-      <c r="AC8" s="6">
-        <v>38.729999999999997</v>
-      </c>
-      <c r="AD8" s="6">
-        <v>41.63</v>
-      </c>
-      <c r="AE8" s="6">
-        <v>44.83</v>
-      </c>
-      <c r="AF8" s="6">
-        <v>47.72</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="6">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="C9" s="6">
-        <v>8.08</v>
-      </c>
-      <c r="D9" s="6">
-        <v>8.59</v>
-      </c>
-      <c r="E9" s="6">
-        <v>9.43</v>
-      </c>
-      <c r="F9" s="6">
-        <v>10.43</v>
-      </c>
-      <c r="G9" s="6">
-        <v>11.61</v>
-      </c>
-      <c r="H9" s="6">
-        <v>12.95</v>
-      </c>
-      <c r="I9" s="6">
-        <v>14.27</v>
-      </c>
-      <c r="J9" s="6">
-        <v>15.65</v>
-      </c>
-      <c r="K9" s="6">
-        <v>17.22</v>
-      </c>
-      <c r="L9" s="6">
-        <v>18.66</v>
-      </c>
-      <c r="M9" s="6">
-        <v>20.11</v>
-      </c>
-      <c r="N9" s="6">
-        <v>21.61</v>
-      </c>
-      <c r="O9" s="6">
-        <v>23.14</v>
-      </c>
-      <c r="P9" s="6">
-        <v>24.54</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>25.95</v>
-      </c>
-      <c r="R9" s="6">
-        <v>27.32</v>
-      </c>
-      <c r="S9" s="6">
-        <v>28.49</v>
-      </c>
-      <c r="T9" s="6">
-        <v>29.5</v>
-      </c>
-      <c r="U9" s="6">
-        <v>30.32</v>
-      </c>
-      <c r="V9" s="6">
-        <v>30.55</v>
-      </c>
-      <c r="W9" s="6">
-        <v>29.64</v>
-      </c>
-      <c r="X9" s="6">
-        <v>20.21</v>
-      </c>
-      <c r="Y9" s="6">
-        <v>22.78</v>
-      </c>
-      <c r="Z9" s="6">
-        <v>27</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>30.57</v>
-      </c>
-      <c r="AB9" s="6">
-        <v>33.89</v>
-      </c>
-      <c r="AC9" s="6">
-        <v>36.79</v>
-      </c>
-      <c r="AD9" s="6">
-        <v>39.549999999999997</v>
-      </c>
-      <c r="AE9" s="6">
-        <v>42.45</v>
-      </c>
-      <c r="AF9" s="6">
-        <v>44.93</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
-        <v>5.0199999999999996</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5.88</v>
-      </c>
-      <c r="D10" s="6">
-        <v>6.98</v>
-      </c>
-      <c r="E10" s="6">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="F10" s="6">
-        <v>9.59</v>
-      </c>
-      <c r="G10" s="6">
-        <v>11.04</v>
-      </c>
-      <c r="H10" s="6">
-        <v>12.59</v>
-      </c>
-      <c r="I10" s="6">
-        <v>14.1</v>
-      </c>
-      <c r="J10" s="6">
-        <v>15.64</v>
-      </c>
-      <c r="K10" s="6">
-        <v>17.39</v>
-      </c>
-      <c r="L10" s="6">
-        <v>18.989999999999998</v>
-      </c>
-      <c r="M10" s="6">
-        <v>20.62</v>
-      </c>
-      <c r="N10" s="6">
-        <v>22.33</v>
-      </c>
-      <c r="O10" s="6">
-        <v>24.12</v>
-      </c>
-      <c r="P10" s="6">
-        <v>25.8</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>27.75</v>
-      </c>
-      <c r="R10" s="6">
-        <v>29.81</v>
-      </c>
-      <c r="S10" s="6">
-        <v>31.74</v>
-      </c>
-      <c r="T10" s="6">
-        <v>33.659999999999997</v>
-      </c>
-      <c r="U10" s="6">
-        <v>35.76</v>
-      </c>
-      <c r="V10" s="6">
-        <v>37.57</v>
-      </c>
-      <c r="W10" s="6">
-        <v>38.78</v>
-      </c>
-      <c r="X10" s="6">
-        <v>16.91</v>
-      </c>
-      <c r="Y10" s="6">
-        <v>20.86</v>
-      </c>
-      <c r="Z10" s="6">
-        <v>25.36</v>
-      </c>
-      <c r="AA10" s="6">
-        <v>29.69</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>33.64</v>
-      </c>
-      <c r="AC10" s="6">
-        <v>37.07</v>
-      </c>
-      <c r="AD10" s="6">
-        <v>40.35</v>
-      </c>
-      <c r="AE10" s="6">
-        <v>43.86</v>
-      </c>
-      <c r="AF10" s="6">
-        <v>46.97</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
@@ -3229,127 +2602,127 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" ref="B19:Q22" si="0">B7-B13</f>
-        <v>-0.98</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
-        <v>2.97</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>5.04</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="0"/>
-        <v>6.98</v>
+        <v>0</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="0"/>
-        <v>8.99</v>
+        <v>0</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="0"/>
-        <v>11.06</v>
+        <v>0</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="0"/>
-        <v>14.94</v>
+        <v>0</v>
       </c>
       <c r="K19" s="4">
         <f t="shared" si="0"/>
-        <v>17.079999999999998</v>
+        <v>0</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="0"/>
-        <v>19.02</v>
+        <v>0</v>
       </c>
       <c r="M19" s="4">
         <f t="shared" si="0"/>
-        <v>20.96</v>
+        <v>0</v>
       </c>
       <c r="N19" s="4">
         <f t="shared" si="0"/>
-        <v>22.97</v>
+        <v>0</v>
       </c>
       <c r="O19" s="4">
         <f t="shared" si="0"/>
-        <v>25.04</v>
+        <v>0</v>
       </c>
       <c r="P19" s="4">
         <f t="shared" si="0"/>
-        <v>26.98</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="0"/>
-        <v>28.99</v>
+        <v>0</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" ref="C19:AF22" si="1">R7-R13</f>
-        <v>31.06</v>
+        <v>0</v>
       </c>
       <c r="S19" s="4">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="T19" s="4">
         <f t="shared" si="1"/>
-        <v>34.94</v>
+        <v>0</v>
       </c>
       <c r="U19" s="4">
         <f t="shared" si="1"/>
-        <v>37.08</v>
+        <v>0</v>
       </c>
       <c r="V19" s="4">
         <f t="shared" si="1"/>
-        <v>39.020000000000003</v>
+        <v>0</v>
       </c>
       <c r="W19" s="4">
         <f t="shared" si="1"/>
-        <v>40.96</v>
+        <v>0</v>
       </c>
       <c r="X19" s="4">
         <f t="shared" si="1"/>
-        <v>42.97</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="4">
         <f t="shared" si="1"/>
-        <v>18.18</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="4">
         <f t="shared" si="1"/>
-        <v>23.57</v>
+        <v>0</v>
       </c>
       <c r="AA19" s="4">
         <f t="shared" si="1"/>
-        <v>27.9</v>
+        <v>0</v>
       </c>
       <c r="AB19" s="4">
         <f t="shared" si="1"/>
-        <v>31.85</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="4">
         <f t="shared" si="1"/>
-        <v>35.28</v>
+        <v>0</v>
       </c>
       <c r="AD19" s="4">
         <f t="shared" si="1"/>
-        <v>38.56</v>
+        <v>0</v>
       </c>
       <c r="AE19" s="4">
         <f t="shared" si="1"/>
-        <v>42.07</v>
+        <v>0</v>
       </c>
       <c r="AF19" s="4">
         <f t="shared" si="1"/>
-        <v>45.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.35">
@@ -3358,127 +2731,127 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" si="0"/>
-        <v>-0.17</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>1.28</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="1"/>
-        <v>2.94</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
-        <v>4.7699999999999996</v>
+        <v>0</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" si="1"/>
-        <v>6.56</v>
+        <v>0</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="1"/>
-        <v>8.4600000000000009</v>
+        <v>0</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="1"/>
-        <v>10.47</v>
+        <v>0</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="1"/>
-        <v>12.37</v>
+        <v>0</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="1"/>
-        <v>14.28</v>
+        <v>0</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="1"/>
-        <v>16.41</v>
+        <v>0</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>18.34</v>
+        <v>0</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="1"/>
-        <v>20.27</v>
+        <v>0</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="1"/>
-        <v>22.27</v>
+        <v>0</v>
       </c>
       <c r="O20" s="4">
         <f t="shared" si="1"/>
-        <v>24.35</v>
+        <v>0</v>
       </c>
       <c r="P20" s="4">
         <f t="shared" si="1"/>
-        <v>26.28</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="1"/>
-        <v>28.29</v>
+        <v>0</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="1"/>
-        <v>30.36</v>
+        <v>0</v>
       </c>
       <c r="S20" s="4">
         <f t="shared" si="1"/>
-        <v>32.299999999999997</v>
+        <v>0</v>
       </c>
       <c r="T20" s="4">
         <f t="shared" si="1"/>
-        <v>34.24</v>
+        <v>0</v>
       </c>
       <c r="U20" s="4">
         <f t="shared" si="1"/>
-        <v>36.29</v>
+        <v>0</v>
       </c>
       <c r="V20" s="4">
         <f t="shared" si="1"/>
-        <v>33.17</v>
+        <v>0</v>
       </c>
       <c r="W20" s="4">
         <f t="shared" si="1"/>
-        <v>29.28</v>
+        <v>0</v>
       </c>
       <c r="X20" s="4">
         <f t="shared" si="1"/>
-        <v>24.22</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="4">
         <f t="shared" si="1"/>
-        <v>26.88</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="4">
         <f t="shared" si="1"/>
-        <v>29.76</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="4">
         <f t="shared" si="1"/>
-        <v>32.75</v>
+        <v>0</v>
       </c>
       <c r="AB20" s="4">
         <f t="shared" si="1"/>
-        <v>35.840000000000003</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="4">
         <f t="shared" si="1"/>
-        <v>38.729999999999997</v>
+        <v>0</v>
       </c>
       <c r="AD20" s="4">
         <f t="shared" si="1"/>
-        <v>41.63</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="4">
         <f t="shared" si="1"/>
-        <v>44.83</v>
+        <v>0</v>
       </c>
       <c r="AF20" s="4">
         <f t="shared" si="1"/>
-        <v>47.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.35">
@@ -3487,127 +2860,127 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" si="0"/>
-        <v>8.0500000000000007</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>8.08</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="1"/>
-        <v>8.59</v>
+        <v>0</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
-        <v>9.43</v>
+        <v>0</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="1"/>
-        <v>10.43</v>
+        <v>0</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="1"/>
-        <v>11.61</v>
+        <v>0</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="1"/>
-        <v>12.95</v>
+        <v>0</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="1"/>
-        <v>14.27</v>
+        <v>0</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="1"/>
-        <v>15.65</v>
+        <v>0</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="1"/>
-        <v>17.22</v>
+        <v>0</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>18.66</v>
+        <v>0</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="1"/>
-        <v>20.11</v>
+        <v>0</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="1"/>
-        <v>21.61</v>
+        <v>0</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="1"/>
-        <v>23.14</v>
+        <v>0</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="1"/>
-        <v>24.54</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="1"/>
-        <v>25.95</v>
+        <v>0</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="1"/>
-        <v>27.32</v>
+        <v>0</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="1"/>
-        <v>28.49</v>
+        <v>0</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="1"/>
-        <v>29.5</v>
+        <v>0</v>
       </c>
       <c r="U21" s="4">
         <f t="shared" si="1"/>
-        <v>30.32</v>
+        <v>0</v>
       </c>
       <c r="V21" s="4">
         <f t="shared" si="1"/>
-        <v>30.55</v>
+        <v>0</v>
       </c>
       <c r="W21" s="4">
         <f t="shared" si="1"/>
-        <v>29.64</v>
+        <v>0</v>
       </c>
       <c r="X21" s="4">
         <f t="shared" si="1"/>
-        <v>20.21</v>
+        <v>0</v>
       </c>
       <c r="Y21" s="4">
         <f t="shared" si="1"/>
-        <v>22.78</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="AA21" s="4">
         <f t="shared" si="1"/>
-        <v>30.57</v>
+        <v>0</v>
       </c>
       <c r="AB21" s="4">
         <f t="shared" si="1"/>
-        <v>33.89</v>
+        <v>0</v>
       </c>
       <c r="AC21" s="4">
         <f t="shared" si="1"/>
-        <v>36.79</v>
+        <v>0</v>
       </c>
       <c r="AD21" s="4">
         <f t="shared" si="1"/>
-        <v>39.549999999999997</v>
+        <v>0</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" si="1"/>
-        <v>42.45</v>
+        <v>0</v>
       </c>
       <c r="AF21" s="4">
         <f t="shared" si="1"/>
-        <v>44.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.35">
@@ -3616,127 +2989,127 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" si="0"/>
-        <v>5.0199999999999996</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>5.88</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="1"/>
-        <v>6.98</v>
+        <v>0</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
-        <v>8.2799999999999994</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" si="1"/>
-        <v>9.59</v>
+        <v>0</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="1"/>
-        <v>11.04</v>
+        <v>0</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="1"/>
-        <v>12.59</v>
+        <v>0</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="1"/>
-        <v>14.1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="1"/>
-        <v>15.64</v>
+        <v>0</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" si="1"/>
-        <v>17.39</v>
+        <v>0</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>18.989999999999998</v>
+        <v>0</v>
       </c>
       <c r="M22" s="4">
         <f t="shared" si="1"/>
-        <v>20.62</v>
+        <v>0</v>
       </c>
       <c r="N22" s="4">
         <f t="shared" si="1"/>
-        <v>22.33</v>
+        <v>0</v>
       </c>
       <c r="O22" s="4">
         <f t="shared" si="1"/>
-        <v>24.12</v>
+        <v>0</v>
       </c>
       <c r="P22" s="4">
         <f t="shared" si="1"/>
-        <v>25.8</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="1"/>
-        <v>27.75</v>
+        <v>0</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="1"/>
-        <v>29.81</v>
+        <v>0</v>
       </c>
       <c r="S22" s="4">
         <f t="shared" si="1"/>
-        <v>31.74</v>
+        <v>0</v>
       </c>
       <c r="T22" s="4">
         <f t="shared" si="1"/>
-        <v>33.659999999999997</v>
+        <v>0</v>
       </c>
       <c r="U22" s="4">
         <f t="shared" si="1"/>
-        <v>35.76</v>
+        <v>0</v>
       </c>
       <c r="V22" s="4">
         <f t="shared" si="1"/>
-        <v>37.57</v>
+        <v>0</v>
       </c>
       <c r="W22" s="4">
         <f t="shared" si="1"/>
-        <v>38.78</v>
+        <v>0</v>
       </c>
       <c r="X22" s="4">
         <f t="shared" si="1"/>
-        <v>16.91</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="4">
         <f t="shared" si="1"/>
-        <v>20.86</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="4">
         <f t="shared" si="1"/>
-        <v>25.36</v>
+        <v>0</v>
       </c>
       <c r="AA22" s="4">
         <f t="shared" si="1"/>
-        <v>29.69</v>
+        <v>0</v>
       </c>
       <c r="AB22" s="4">
         <f t="shared" si="1"/>
-        <v>33.64</v>
+        <v>0</v>
       </c>
       <c r="AC22" s="4">
         <f t="shared" si="1"/>
-        <v>37.07</v>
+        <v>0</v>
       </c>
       <c r="AD22" s="4">
         <f t="shared" si="1"/>
-        <v>40.35</v>
+        <v>0</v>
       </c>
       <c r="AE22" s="4">
         <f t="shared" si="1"/>
-        <v>43.86</v>
+        <v>0</v>
       </c>
       <c r="AF22" s="4">
         <f t="shared" si="1"/>
-        <v>46.97</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>